<commit_message>
fix automatic input of variables 0.1.6.0
</commit_message>
<xml_diff>
--- a/УЛЬТИМАТИВНАЯ_Формулы.xlsx
+++ b/УЛЬТИМАТИВНАЯ_Формулы.xlsx
@@ -444,22 +444,22 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>8-осный</t>
+          <t>8-миосный</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>8-осный</t>
+          <t>8-миосный</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>8-осный</t>
+          <t>8-миосный</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>8-осный</t>
+          <t>8-миосный</t>
         </is>
       </c>
     </row>
@@ -605,16 +605,16 @@
         <v>3160</v>
       </c>
       <c r="E6" t="n">
-        <v>3160</v>
+        <v>995</v>
       </c>
       <c r="F6" t="n">
-        <v>3160</v>
+        <v>995</v>
       </c>
       <c r="G6" t="n">
-        <v>3160</v>
+        <v>995</v>
       </c>
       <c r="H6" t="n">
-        <v>3160</v>
+        <v>995</v>
       </c>
     </row>
     <row r="7">
@@ -657,16 +657,16 @@
         <v>125</v>
       </c>
       <c r="E8" t="n">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="F8" t="n">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="G8" t="n">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="H8" t="n">
-        <v>125</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
@@ -683,16 +683,16 @@
         <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -748,19 +748,19 @@
         <v>1.33</v>
       </c>
       <c r="D11" t="n">
-        <v>1.25</v>
+        <v>1.33</v>
       </c>
       <c r="E11" t="n">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="F11" t="n">
-        <v>1.33</v>
+        <v>1.18</v>
       </c>
       <c r="G11" t="n">
-        <v>1.25</v>
+        <v>1.37</v>
       </c>
       <c r="H11" t="n">
-        <v>1.33</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="12">
@@ -777,16 +777,16 @@
         <v>0.047</v>
       </c>
       <c r="E12" t="n">
-        <v>0.047</v>
+        <v>0.067</v>
       </c>
       <c r="F12" t="n">
-        <v>0.047</v>
+        <v>0.067</v>
       </c>
       <c r="G12" t="n">
-        <v>0.047</v>
+        <v>0.067</v>
       </c>
       <c r="H12" t="n">
-        <v>0.047</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="13">
@@ -854,22 +854,22 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>185+125+185</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>185+125+185</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>185+125+185</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>185+125+185</t>
         </is>
       </c>
     </row>
@@ -943,54 +943,54 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1840</v>
+        <v>260</v>
       </c>
       <c r="B17" t="n">
-        <v>1840</v>
+        <v>500</v>
       </c>
       <c r="C17" t="n">
+        <v>290</v>
+      </c>
+      <c r="D17" t="n">
+        <v>600</v>
+      </c>
+      <c r="E17" t="n">
         <v>260</v>
       </c>
-      <c r="D17" t="n">
-        <v>1840</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1840</v>
-      </c>
       <c r="F17" t="n">
-        <v>260</v>
+        <v>500</v>
       </c>
       <c r="G17" t="n">
-        <v>1840</v>
+        <v>290</v>
       </c>
       <c r="H17" t="n">
-        <v>260</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.01176</v>
+        <v>0.01145</v>
       </c>
       <c r="B18" t="n">
         <v>0.01311</v>
       </c>
       <c r="C18" t="n">
+        <v>0.01176</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.01372</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.01145</v>
       </c>
-      <c r="D18" t="n">
+      <c r="F18" t="n">
+        <v>0.01311</v>
+      </c>
+      <c r="G18" t="n">
         <v>0.01176</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.01311</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.01145</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.01311</v>
-      </c>
       <c r="H18" t="n">
-        <v>0.01145</v>
+        <v>0.01372</v>
       </c>
     </row>
     <row r="19">
@@ -1255,288 +1255,288 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>7108.12</v>
+        <v>2707.91</v>
       </c>
       <c r="B29" t="n">
-        <v>6732.2</v>
+        <v>3509.4</v>
       </c>
       <c r="C29" t="n">
-        <v>2920.29</v>
+        <v>3043.25</v>
       </c>
       <c r="D29" t="n">
-        <v>7665.62</v>
+        <v>4052.66</v>
       </c>
       <c r="E29" t="n">
-        <v>8459.459999999999</v>
+        <v>1909.36</v>
       </c>
       <c r="F29" t="n">
-        <v>3402.66</v>
+        <v>2474.5</v>
       </c>
       <c r="G29" t="n">
-        <v>9122.950000000001</v>
+        <v>2145.81</v>
       </c>
       <c r="H29" t="n">
-        <v>3669.54</v>
+        <v>2857.55</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>239.52</v>
+        <v>119.32</v>
       </c>
       <c r="B30" t="n">
-        <v>227.78</v>
+        <v>133.78</v>
       </c>
       <c r="C30" t="n">
-        <v>119.32</v>
+        <v>120.45</v>
       </c>
       <c r="D30" t="n">
-        <v>239.52</v>
+        <v>139.98</v>
       </c>
       <c r="E30" t="n">
-        <v>227.78</v>
+        <v>92.54000000000001</v>
       </c>
       <c r="F30" t="n">
-        <v>119.32</v>
+        <v>116.09</v>
       </c>
       <c r="G30" t="n">
-        <v>227.78</v>
+        <v>95.81</v>
       </c>
       <c r="H30" t="n">
-        <v>119.32</v>
+        <v>123.57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4680.73</v>
+        <v>679.3099999999999</v>
       </c>
       <c r="B31" t="n">
-        <v>4198.73</v>
+        <v>1140.96</v>
       </c>
       <c r="C31" t="n">
-        <v>679.3099999999999</v>
+        <v>737.72</v>
       </c>
       <c r="D31" t="n">
-        <v>4680.73</v>
+        <v>1308.28</v>
       </c>
       <c r="E31" t="n">
-        <v>4198.73</v>
+        <v>968.38</v>
       </c>
       <c r="F31" t="n">
-        <v>679.3099999999999</v>
+        <v>1626.47</v>
       </c>
       <c r="G31" t="n">
-        <v>4198.73</v>
+        <v>1051.65</v>
       </c>
       <c r="H31" t="n">
-        <v>679.3099999999999</v>
+        <v>1864.99</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7190.46</v>
+        <v>2719.7</v>
       </c>
       <c r="B32" t="n">
-        <v>6802.99</v>
+        <v>3524.96</v>
       </c>
       <c r="C32" t="n">
-        <v>2931.23</v>
+        <v>3054.47</v>
       </c>
       <c r="D32" t="n">
-        <v>7742.03</v>
+        <v>4068.86</v>
       </c>
       <c r="E32" t="n">
-        <v>8518.139999999999</v>
+        <v>1940.68</v>
       </c>
       <c r="F32" t="n">
-        <v>3417.64</v>
+        <v>2516.7</v>
       </c>
       <c r="G32" t="n">
-        <v>9177.389999999999</v>
+        <v>2175.79</v>
       </c>
       <c r="H32" t="n">
-        <v>3683.43</v>
+        <v>2901.65</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>31027.89</v>
+        <v>19850.99</v>
       </c>
       <c r="B33" t="n">
-        <v>30059.21</v>
+        <v>21864.14</v>
       </c>
       <c r="C33" t="n">
-        <v>20379.81</v>
+        <v>20687.92</v>
       </c>
       <c r="D33" t="n">
-        <v>32406.82</v>
+        <v>23223.89</v>
       </c>
       <c r="E33" t="n">
-        <v>37695.73</v>
+        <v>21252.08</v>
       </c>
       <c r="F33" t="n">
-        <v>24944.48</v>
+        <v>22692.13</v>
       </c>
       <c r="G33" t="n">
-        <v>39343.85</v>
+        <v>21839.86</v>
       </c>
       <c r="H33" t="n">
-        <v>25608.96</v>
+        <v>23654.51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>66.75</v>
+        <v>68.56</v>
       </c>
       <c r="B34" t="n">
         <v>59.88</v>
       </c>
       <c r="C34" t="n">
+        <v>66.75</v>
+      </c>
+      <c r="D34" t="n">
+        <v>57.22</v>
+      </c>
+      <c r="E34" t="n">
         <v>68.56</v>
       </c>
-      <c r="D34" t="n">
+      <c r="F34" t="n">
+        <v>59.88</v>
+      </c>
+      <c r="G34" t="n">
         <v>66.75</v>
       </c>
-      <c r="E34" t="n">
-        <v>59.88</v>
-      </c>
-      <c r="F34" t="n">
-        <v>68.56</v>
-      </c>
-      <c r="G34" t="n">
-        <v>59.88</v>
-      </c>
       <c r="H34" t="n">
-        <v>68.56</v>
+        <v>57.22</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>333.76</v>
+        <v>342.79</v>
       </c>
       <c r="B35" t="n">
         <v>299.39</v>
       </c>
       <c r="C35" t="n">
+        <v>333.76</v>
+      </c>
+      <c r="D35" t="n">
+        <v>286.08</v>
+      </c>
+      <c r="E35" t="n">
         <v>342.79</v>
       </c>
-      <c r="D35" t="n">
+      <c r="F35" t="n">
+        <v>299.39</v>
+      </c>
+      <c r="G35" t="n">
         <v>333.76</v>
       </c>
-      <c r="E35" t="n">
-        <v>299.39</v>
-      </c>
-      <c r="F35" t="n">
-        <v>342.79</v>
-      </c>
-      <c r="G35" t="n">
-        <v>299.39</v>
-      </c>
       <c r="H35" t="n">
-        <v>342.79</v>
+        <v>286.08</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>200.26</v>
+        <v>205.68</v>
       </c>
       <c r="B36" t="n">
         <v>179.63</v>
       </c>
       <c r="C36" t="n">
+        <v>200.26</v>
+      </c>
+      <c r="D36" t="n">
+        <v>171.65</v>
+      </c>
+      <c r="E36" t="n">
         <v>205.68</v>
       </c>
-      <c r="D36" t="n">
+      <c r="F36" t="n">
+        <v>179.63</v>
+      </c>
+      <c r="G36" t="n">
         <v>200.26</v>
       </c>
-      <c r="E36" t="n">
-        <v>179.63</v>
-      </c>
-      <c r="F36" t="n">
-        <v>205.68</v>
-      </c>
-      <c r="G36" t="n">
-        <v>179.63</v>
-      </c>
       <c r="H36" t="n">
-        <v>205.68</v>
+        <v>171.65</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>467.26</v>
+        <v>479.91</v>
       </c>
       <c r="B37" t="n">
         <v>419.15</v>
       </c>
       <c r="C37" t="n">
+        <v>467.26</v>
+      </c>
+      <c r="D37" t="n">
+        <v>400.51</v>
+      </c>
+      <c r="E37" t="n">
         <v>479.91</v>
       </c>
-      <c r="D37" t="n">
+      <c r="F37" t="n">
+        <v>419.15</v>
+      </c>
+      <c r="G37" t="n">
         <v>467.26</v>
       </c>
-      <c r="E37" t="n">
-        <v>419.15</v>
-      </c>
-      <c r="F37" t="n">
-        <v>479.91</v>
-      </c>
-      <c r="G37" t="n">
-        <v>419.15</v>
-      </c>
       <c r="H37" t="n">
-        <v>479.91</v>
+        <v>400.51</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>30817.33</v>
+        <v>19570.01</v>
       </c>
       <c r="B38" t="n">
-        <v>30061.38</v>
+        <v>21866.31</v>
       </c>
       <c r="C38" t="n">
-        <v>20098.83</v>
+        <v>20477.36</v>
       </c>
       <c r="D38" t="n">
-        <v>32196.26</v>
+        <v>23280.45</v>
       </c>
       <c r="E38" t="n">
-        <v>37698.46</v>
+        <v>18375.12</v>
       </c>
       <c r="F38" t="n">
-        <v>24591.41</v>
+        <v>20719.37</v>
       </c>
       <c r="G38" t="n">
-        <v>39346.58</v>
+        <v>19146.32</v>
       </c>
       <c r="H38" t="n">
-        <v>25255.89</v>
+        <v>21965.09</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-0.01613</v>
+        <v>-0.02153</v>
       </c>
       <c r="B39" t="n">
         <v>0.00017</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.02153</v>
+        <v>-0.01613</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.01613</v>
+        <v>0.00433</v>
       </c>
       <c r="E39" t="n">
-        <v>0.00017</v>
+        <v>-0.16526</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.02153</v>
+        <v>-0.12478</v>
       </c>
       <c r="G39" t="n">
-        <v>0.00017</v>
+        <v>-0.15796</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.02153</v>
+        <v>-0.10989</v>
       </c>
     </row>
     <row r="40">
@@ -1553,16 +1553,16 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>-0.01498</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>0.00332</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>-0.01025</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>0.00644</v>
       </c>
     </row>
     <row r="41">
@@ -1593,80 +1593,80 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-0.01613</v>
+        <v>-0.02153</v>
       </c>
       <c r="B42" t="n">
         <v>0.00017</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.02153</v>
+        <v>-0.01613</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.01613</v>
+        <v>0.00433</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00017</v>
+        <v>-0.18024</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.02153</v>
+        <v>-0.12146</v>
       </c>
       <c r="G42" t="n">
-        <v>0.00017</v>
+        <v>-0.16821</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.02153</v>
+        <v>-0.10345</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>30528.53</v>
+        <v>19326.7</v>
       </c>
       <c r="B43" t="n">
-        <v>29697.68</v>
+        <v>21502.61</v>
       </c>
       <c r="C43" t="n">
-        <v>19855.52</v>
+        <v>20188.56</v>
       </c>
       <c r="D43" t="n">
-        <v>31907.46</v>
+        <v>22928.27</v>
       </c>
       <c r="E43" t="n">
-        <v>37241.44</v>
+        <v>25716.76</v>
       </c>
       <c r="F43" t="n">
-        <v>24285.68</v>
+        <v>25117.42</v>
       </c>
       <c r="G43" t="n">
-        <v>38889.56</v>
+        <v>25862.22</v>
       </c>
       <c r="H43" t="n">
-        <v>24950.16</v>
+        <v>25507.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>-0.03826</v>
+        <v>-0.04017</v>
       </c>
       <c r="B44" t="n">
         <v>-0.0277</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.04017</v>
+        <v>-0.03826</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.03826</v>
+        <v>-0.02265</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.0277</v>
+        <v>0.04008</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.04017</v>
+        <v>-0.00864</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.0277</v>
+        <v>0.02884</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.04017</v>
+        <v>-0.02022</v>
       </c>
     </row>
     <row r="45">
@@ -1683,16 +1683,16 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>0.26993</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>0.18059</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>0.25189</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>0.15223</v>
       </c>
     </row>
     <row r="46">
@@ -1709,42 +1709,42 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>-0.03778</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>-0.02407</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-0.03547</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>-0.01905</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-0.03826</v>
+        <v>-0.04017</v>
       </c>
       <c r="B47" t="n">
         <v>-0.0277</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.04017</v>
+        <v>-0.03826</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.03826</v>
+        <v>-0.02265</v>
       </c>
       <c r="E47" t="n">
-        <v>-0.0277</v>
+        <v>0.27223</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.04017</v>
+        <v>0.14788</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.0277</v>
+        <v>0.24526</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.04017</v>
+        <v>0.11296</v>
       </c>
     </row>
     <row r="48">
@@ -1761,94 +1761,94 @@
         <v>1</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2999.68</v>
+        <v>1956.47</v>
       </c>
       <c r="B49" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="C49" t="n">
-        <v>2137.93</v>
+        <v>2120.78</v>
       </c>
       <c r="D49" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="E49" t="n">
-        <v>3291.61</v>
+        <v>1734.14</v>
       </c>
       <c r="F49" t="n">
-        <v>2615.81</v>
+        <v>1707.78</v>
       </c>
       <c r="G49" t="n">
-        <v>3435.51</v>
+        <v>2042.57</v>
       </c>
       <c r="H49" t="n">
-        <v>2686.5</v>
+        <v>2008.52</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>17.37</v>
+        <v>10.71</v>
       </c>
       <c r="B50" t="n">
-        <v>18.84</v>
+        <v>13.64</v>
       </c>
       <c r="C50" t="n">
-        <v>11.86</v>
+        <v>12.39</v>
       </c>
       <c r="D50" t="n">
-        <v>19.58</v>
+        <v>16.42</v>
       </c>
       <c r="E50" t="n">
-        <v>23.62</v>
+        <v>14.25</v>
       </c>
       <c r="F50" t="n">
-        <v>13.46</v>
+        <v>15.93</v>
       </c>
       <c r="G50" t="n">
-        <v>26.6</v>
+        <v>15.87</v>
       </c>
       <c r="H50" t="n">
-        <v>14.91</v>
+        <v>18.26</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>3.71</v>
+        <v>2.29</v>
       </c>
       <c r="B51" t="n">
-        <v>4.03</v>
+        <v>2.92</v>
       </c>
       <c r="C51" t="n">
-        <v>2.54</v>
+        <v>2.65</v>
       </c>
       <c r="D51" t="n">
-        <v>4.18</v>
+        <v>3.51</v>
       </c>
       <c r="E51" t="n">
-        <v>5.05</v>
+        <v>3.04</v>
       </c>
       <c r="F51" t="n">
-        <v>2.88</v>
+        <v>3.41</v>
       </c>
       <c r="G51" t="n">
-        <v>5.69</v>
+        <v>3.39</v>
       </c>
       <c r="H51" t="n">
-        <v>3.19</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="52">
@@ -1879,54 +1879,54 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.08</v>
+        <v>1.31</v>
       </c>
       <c r="B55" t="n">
-        <v>1.04</v>
+        <v>1.2</v>
       </c>
       <c r="C55" t="n">
-        <v>1.26</v>
+        <v>1.24</v>
       </c>
       <c r="D55" t="n">
-        <v>1.03</v>
+        <v>1.11</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>1.18</v>
       </c>
       <c r="F55" t="n">
-        <v>1.21</v>
+        <v>1.13</v>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>1.13</v>
       </c>
       <c r="H55" t="n">
-        <v>1.16</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.656</v>
+        <v>0.405</v>
       </c>
       <c r="B56" t="n">
-        <v>0.712</v>
+        <v>0.516</v>
       </c>
       <c r="C56" t="n">
-        <v>0.449</v>
+        <v>0.469</v>
       </c>
       <c r="D56" t="n">
-        <v>0.738</v>
+        <v>0.62</v>
       </c>
       <c r="E56" t="n">
-        <v>0.892</v>
+        <v>0.538</v>
       </c>
       <c r="F56" t="n">
-        <v>0.509</v>
+        <v>0.603</v>
       </c>
       <c r="G56" t="n">
-        <v>1.005</v>
+        <v>0.599</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.6889999999999999</v>
       </c>
     </row>
     <row r="57">
@@ -1995,16 +1995,16 @@
         <v>300</v>
       </c>
       <c r="E59" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="F59" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="G59" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="H59" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60">
@@ -2021,16 +2021,16 @@
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61">
@@ -2047,16 +2047,16 @@
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64">
@@ -2087,28 +2087,28 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B67" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C67" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D67" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="E67" t="n">
-        <v>-11</v>
+        <v>69</v>
       </c>
       <c r="F67" t="n">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="G67" t="n">
-        <v>-18</v>
+        <v>53</v>
       </c>
       <c r="H67" t="n">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68">
@@ -2211,16 +2211,16 @@
         <v>300</v>
       </c>
       <c r="E72" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="F72" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="G72" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
       <c r="H72" t="n">
-        <v>300</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73">
@@ -2237,16 +2237,16 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="H73" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74">
@@ -2263,16 +2263,16 @@
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>495</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>495</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>495</v>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>495</v>
       </c>
     </row>
     <row r="81">
@@ -2289,276 +2289,276 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="H81" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="D82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.01006</v>
+        <v>0.27492</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="B95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="C95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="E95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="G95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="H95" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="B99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="D99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="F99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="G99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
       <c r="H99" t="n">
-        <v>-0.04301</v>
+        <v>0.55906</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="B100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="C100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="D100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="E100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="F100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="G100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
       <c r="H100" t="n">
-        <v>26966.14</v>
+        <v>20931.34</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="B101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="C101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="D101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="E101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="F101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="G101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
       <c r="H101" t="n">
-        <v>27131.12</v>
+        <v>16422.54</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="B102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="C102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="D102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="E102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="F102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="G102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
       <c r="H102" t="n">
-        <v>3.66</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="B103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="C103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="D103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="E103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="F103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="G103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
       <c r="H103" t="n">
-        <v>0.2525</v>
+        <v>0.1711</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="B104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="C104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="D104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="E104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="F104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="G104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
       <c r="H104" t="n">
-        <v>3.678</v>
+        <v>1.944</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="B105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="C105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="D105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="E105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="F105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="G105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
       <c r="H105" t="n">
-        <v>0.2538</v>
+        <v>0.1341</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="B106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="C106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="D106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="E106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="F106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="G106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
       <c r="H106" t="n">
-        <v>1.398</v>
+        <v>0.843</v>
       </c>
     </row>
     <row r="107">
@@ -2615,262 +2615,262 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="E113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="F113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="G113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="H113" t="n">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>4479.184</v>
+        <v>4055.411</v>
       </c>
       <c r="B114" t="n">
-        <v>3991.814</v>
+        <v>3994.012</v>
       </c>
       <c r="C114" t="n">
-        <v>3358.909</v>
+        <v>4269.014000000001</v>
       </c>
       <c r="D114" t="n">
-        <v>4653.67</v>
+        <v>4198.645</v>
       </c>
       <c r="E114" t="n">
-        <v>4858.693000000001</v>
+        <v>3766.382</v>
       </c>
       <c r="F114" t="n">
-        <v>3980.153</v>
+        <v>3732.114</v>
       </c>
       <c r="G114" t="n">
-        <v>5045.763000000001</v>
+        <v>4167.341</v>
       </c>
       <c r="H114" t="n">
-        <v>4072.05</v>
+        <v>4123.076</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="B115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="C115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="D115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="E115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="F115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="G115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
       <c r="H115" t="n">
-        <v>-3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3823.984</v>
+        <v>3853.811</v>
       </c>
       <c r="B116" t="n">
-        <v>3336.614</v>
+        <v>3792.412</v>
       </c>
       <c r="C116" t="n">
-        <v>2703.709</v>
+        <v>4067.414000000001</v>
       </c>
       <c r="D116" t="n">
-        <v>3998.47</v>
+        <v>3997.045</v>
       </c>
       <c r="E116" t="n">
-        <v>4203.493</v>
+        <v>3564.782</v>
       </c>
       <c r="F116" t="n">
-        <v>3324.953</v>
+        <v>3530.514</v>
       </c>
       <c r="G116" t="n">
-        <v>4390.563</v>
+        <v>3965.741</v>
       </c>
       <c r="H116" t="n">
-        <v>3416.85</v>
+        <v>3921.476</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="B117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="C117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="D117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="E117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="F117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="G117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
       <c r="H117" t="n">
-        <v>579.6</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="B118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="C118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="D118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="E118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="F118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="G118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
       <c r="H118" t="n">
-        <v>-75.59999999999999</v>
+        <v>1310.4</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="B119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="C119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="D119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="E119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="F119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="G119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
       <c r="H119" t="n">
-        <v>3991.81</v>
+        <v>3994.01</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="B120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="C120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="D120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="E120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="F120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="G120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
       <c r="H120" t="n">
-        <v>3998.47</v>
+        <v>3997.04</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="B121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="C121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="D121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="E121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="F121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="G121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
       <c r="H121" t="n">
-        <v>2624.78</v>
+        <v>1909.24</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="B122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="C122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="D122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="E122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="F122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="G122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
       <c r="H122" t="n">
-        <v>3133.9</v>
+        <v>2066.65</v>
       </c>
     </row>
     <row r="123">
@@ -3136,120 +3136,153 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
+          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; η = -0.04017
+III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; η = 0</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; η = -0.0277
+III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; η = 0</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
           <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; η = -0.03826
 III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; η = 0
 VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; η = 0</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; η = -0.0277
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; η = 0</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; η = -0.04017
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; η = 0</t>
-        </is>
-      </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; η = -0.03826
-III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; η = 0</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; η = -0.0277
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; η = 0</t>
+          <t>I ось: x = 185 см; kx = 0.01145×185 = 2.12; η = 0.04008
+III ось: x = 125 см; kx = 0.01145×125 = 1.43; η = 0.26993
+VI ось: x = 125+185 см; kx = 0.01145×310 = 3.55; η = -0.03778</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; η = -0.04017
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; η = 0</t>
+          <t>I ось: x = 185 см; kx = 0.01311×185 = 2.43; η = -0.00864
+III ось: x = 125 см; kx = 0.01311×125 = 1.64; η = 0.18059
+VI ось: x = 125+185 см; kx = 0.01311×310 = 4.06; η = -0.02407</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; η = -0.0277
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; η = 0</t>
+          <t>I ось: x = 185 см; kx = 0.01176×185 = 2.18; η = 0.02884
+III ось: x = 125 см; kx = 0.01176×125 = 1.47; η = 0.25189
+VI ось: x = 125+185 см; kx = 0.01176×310 = 3.65; η = -0.03547</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; η = -0.04017
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; η = 0</t>
+          <t>I ось: x = 185 см; kx = 0.01372×185 = 2.54; η = -0.02022
+III ось: x = 125 см; kx = 0.01372×125 = 1.71; η = 0.15223
+VI ось: x = 125+185 см; kx = 0.01372×310 = 4.25; η = -0.01905</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; µ = -0.02153
+III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; µ = 0.00000</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; µ = 0.00017
+III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; µ = 0.00000</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
         <is>
           <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; µ = -0.01613
 III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; µ = 0.00000
 VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; µ = 0.00000</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; µ = 0.00017
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; µ = 0.00000</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; µ = -0.02153
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; µ = 0.00000</t>
-        </is>
-      </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; µ = -0.01613
-III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; µ = 0.00000</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; µ = 0.00017
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; µ = 0.00000</t>
+          <t>II ось: x = 185 см; kx = 0.01145×185 = 2.12; µ = -0.16526
+III ось: x = 125+185 см; kx = 0.01145×310 = 3.55; µ = -0.01498
+VI ось: x = 185+125+185 см; kx = 0.01145×495 = 5.67; µ = 0.00000</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; µ = -0.02153
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; µ = 0.00000</t>
+          <t>II ось: x = 185 см; kx = 0.01311×185 = 2.43; µ = -0.12478
+III ось: x = 125+185 см; kx = 0.01311×310 = 4.06; µ = 0.00332
+VI ось: x = 185+125+185 см; kx = 0.01311×495 = 6.49; µ = 0.00000</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; µ = 0.00017
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; µ = 0.00000</t>
+          <t>II ось: x = 185 см; kx = 0.01176×185 = 2.18; µ = -0.15796
+III ось: x = 125+185 см; kx = 0.01176×310 = 3.65; µ = -0.01025
+VI ось: x = 185+125+185 см; kx = 0.01176×495 = 5.82; µ = 0.00000</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; µ = -0.02153
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; µ = 0.00000</t>
-        </is>
-      </c>
-    </row>
-    <row r="135"/>
+          <t>II ось: x = 185 см; kx = 0.01372×185 = 2.54; µ = -0.10989
+III ось: x = 125+185 см; kx = 0.01372×310 = 4.25; µ = 0.00644
+VI ось: x = 185+125+185 см; kx = 0.01372×495 = 6.79; µ = 0.00000</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>ηI: x = 185 - 55 см; kx = 0.01145×130 = 1.49; η = 0.04008
+ηII: x = 55 см; kx = 0.01145×55 = 0.63; η = 0.74428
+ηIII: x = 125+55 см; kx = 0.01145×180 = 56.43; η = 0.05239
+ηIV: x = 125+185+55; kx = 0.01145×365 = 3.61; η = -0.02097</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>ηI: x = 185 - 55 см; kx = 0.01311×130 = 1.70; η = -0.00864
+ηII: x = 55 см; kx = 0.01311×55 = 0.72; η = 0.68623
+ηIII: x = 125+55 см; kx = 0.01311×180 = 56.64; η = -0.00048
+ηIV: x = 125+185+55; kx = 0.01311×365 = 4.13; η = -0.00772</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>ηI: x = 185 - 55 см; kx = 0.01176×130 = 1.53; η = 0.02884
+ηII: x = 55 см; kx = 0.01176×55 = 0.65; η = 0.73355
+ηIII: x = 125+55 см; kx = 0.01176×180 = 56.47; η = 0.04038
+ηIV: x = 125+185+55; kx = 0.01176×365 = 3.70; η = -0.01806</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>ηI: x = 185 - 55 см; kx = 0.01372×130 = 1.78; η = -0.02022
+ηII: x = 55 см; kx = 0.01372×55 = 0.75; η = 0.66465
+ηIII: x = 125+55 см; kx = 0.01372×180 = 56.72; η = -0.01354
+ηIV: x = 125+185+55; kx = 0.01372×365 = 4.32; η = -0.00445</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix excel input of variables 0.1.7.0
</commit_message>
<xml_diff>
--- a/УЛЬТИМАТИВНАЯ_Формулы.xlsx
+++ b/УЛЬТИМАТИВНАЯ_Формулы.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,42 +422,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>ВЛ10</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ВЛ10</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ВЛ10</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>ВЛ10</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>8-миосный</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>8-миосный</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>8-миосный</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>8-миосный</t>
         </is>
@@ -540,144 +510,82 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11500</v>
-      </c>
-      <c r="B4" t="n">
-        <v>11500</v>
-      </c>
-      <c r="C4" t="n">
-        <v>11500</v>
-      </c>
       <c r="D4" t="n">
         <v>11500</v>
       </c>
       <c r="E4" t="n">
         <v>14000</v>
       </c>
-      <c r="F4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="G4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="H4" t="n">
-        <v>14000</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pcт</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>85</v>
       </c>
-      <c r="B5" t="n">
-        <v>85</v>
-      </c>
-      <c r="C5" t="n">
-        <v>85</v>
-      </c>
-      <c r="D5" t="n">
-        <v>85</v>
-      </c>
-      <c r="E5" t="n">
-        <v>85</v>
-      </c>
-      <c r="F5" t="n">
-        <v>85</v>
-      </c>
-      <c r="G5" t="n">
-        <v>85</v>
-      </c>
-      <c r="H5" t="n">
-        <v>85</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Скорость</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>3160</v>
-      </c>
-      <c r="B6" t="n">
-        <v>3160</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3160</v>
-      </c>
       <c r="D6" t="n">
         <v>3160</v>
       </c>
       <c r="E6" t="n">
         <v>995</v>
       </c>
-      <c r="F6" t="n">
-        <v>995</v>
-      </c>
-      <c r="G6" t="n">
-        <v>995</v>
-      </c>
-      <c r="H6" t="n">
-        <v>995</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>116</v>
-      </c>
-      <c r="B7" t="n">
-        <v>116</v>
-      </c>
-      <c r="C7" t="n">
-        <v>116</v>
-      </c>
       <c r="D7" t="n">
         <v>116</v>
       </c>
       <c r="E7" t="n">
         <v>200</v>
       </c>
-      <c r="F7" t="n">
-        <v>200</v>
-      </c>
-      <c r="G7" t="n">
-        <v>200</v>
-      </c>
-      <c r="H7" t="n">
-        <v>200</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>JestcostRessor</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>125</v>
-      </c>
-      <c r="B8" t="n">
-        <v>125</v>
-      </c>
-      <c r="C8" t="n">
-        <v>125</v>
-      </c>
       <c r="D8" t="n">
         <v>125</v>
       </c>
       <c r="E8" t="n">
         <v>95</v>
       </c>
-      <c r="F8" t="n">
-        <v>95</v>
-      </c>
-      <c r="G8" t="n">
-        <v>95</v>
-      </c>
-      <c r="H8" t="n">
-        <v>95</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
       </c>
       <c r="D9" t="n">
         <v>2</v>
@@ -685,14 +593,20 @@
       <c r="E9" t="n">
         <v>4</v>
       </c>
-      <c r="F9" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" t="n">
-        <v>4</v>
-      </c>
-      <c r="H9" t="n">
-        <v>4</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -762,54 +676,31 @@
       <c r="H11" t="n">
         <v>1.37</v>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>0.047</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.047</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.047</v>
-      </c>
       <c r="D12" t="n">
         <v>0.047</v>
       </c>
       <c r="E12" t="n">
         <v>0.067</v>
       </c>
-      <c r="F12" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.067</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Электровоз</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Электровоз</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Электровоз</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Электровоз</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>НЕТУ</t>
@@ -817,17 +708,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>НЕТУ</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>НЕТУ</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>НЕТУ</t>
+          <t>z_max</t>
         </is>
       </c>
     </row>
@@ -874,29 +755,16 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>17.84</v>
-      </c>
-      <c r="B15" t="n">
-        <v>17.84</v>
-      </c>
-      <c r="C15" t="n">
-        <v>17.84</v>
-      </c>
       <c r="D15" t="n">
         <v>17.84</v>
       </c>
       <c r="E15" t="n">
         <v>16</v>
       </c>
-      <c r="F15" t="n">
-        <v>16</v>
-      </c>
-      <c r="G15" t="n">
-        <v>16</v>
-      </c>
-      <c r="H15" t="n">
-        <v>16</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>z_max</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -966,6 +834,11 @@
       <c r="H17" t="n">
         <v>600</v>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -992,31 +865,20 @@
       <c r="H18" t="n">
         <v>0.01372</v>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>1</v>
       </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -2110,6 +1972,11 @@
       <c r="H67" t="n">
         <v>55</v>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>[∆t_р]</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2275,6 +2142,66 @@
         <v>495</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2400</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Loko_[бкр]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>20</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Loko_[бш]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Loko_[бб]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Vag_[бкр]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>18</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Vag_[бш]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Vag_[бб]</t>
+        </is>
+      </c>
+    </row>
     <row r="81">
       <c r="A81" t="n">
         <v>0</v>
@@ -2353,32 +2280,6 @@
         <v>0.55906</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="B99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="C99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="E99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="G99" t="n">
-        <v>0.55906</v>
-      </c>
-      <c r="H99" t="n">
-        <v>0.55906</v>
-      </c>
-    </row>
     <row r="100">
       <c r="A100" t="n">
         <v>20931.34</v>
@@ -2586,6 +2487,11 @@
       <c r="H107" t="n">
         <v>2950</v>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>Параметр А Першин</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -2612,6 +2518,11 @@
       <c r="H108" t="n">
         <v>0.365</v>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>Параметр µ Першин</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -2638,31 +2549,41 @@
       <c r="H113" t="n">
         <v>60</v>
       </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>[∆t_р_min]Прямая</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>4055.411</v>
+        <v>3994.01</v>
       </c>
       <c r="B114" t="n">
-        <v>3994.012</v>
+        <v>3994.01</v>
       </c>
       <c r="C114" t="n">
-        <v>4269.014000000001</v>
+        <v>3994.01</v>
       </c>
       <c r="D114" t="n">
-        <v>4198.645</v>
+        <v>3994.01</v>
       </c>
       <c r="E114" t="n">
-        <v>3766.382</v>
+        <v>3994.01</v>
       </c>
       <c r="F114" t="n">
-        <v>3732.114</v>
+        <v>3994.01</v>
       </c>
       <c r="G114" t="n">
-        <v>4167.341</v>
+        <v>3994.01</v>
       </c>
       <c r="H114" t="n">
-        <v>4123.076</v>
+        <v>3994.01</v>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>нормальные суммарные напряжения(Прямая)</t>
+        </is>
       </c>
     </row>
     <row r="115">
@@ -2690,31 +2611,41 @@
       <c r="H115" t="n">
         <v>52</v>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>[∆t_р_min]Кривая</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3853.811</v>
+        <v>3997.04</v>
       </c>
       <c r="B116" t="n">
-        <v>3792.412</v>
+        <v>3997.04</v>
       </c>
       <c r="C116" t="n">
-        <v>4067.414000000001</v>
+        <v>3997.04</v>
       </c>
       <c r="D116" t="n">
-        <v>3997.045</v>
+        <v>3997.04</v>
       </c>
       <c r="E116" t="n">
-        <v>3564.782</v>
+        <v>3997.04</v>
       </c>
       <c r="F116" t="n">
-        <v>3530.514</v>
+        <v>3997.04</v>
       </c>
       <c r="G116" t="n">
-        <v>3965.741</v>
+        <v>3997.04</v>
       </c>
       <c r="H116" t="n">
-        <v>3921.476</v>
+        <v>3997.04</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>нормальные суммарные напряжения(Кривая)</t>
+        </is>
       </c>
     </row>
     <row r="117">
@@ -2742,6 +2673,11 @@
       <c r="H117" t="n">
         <v>1512</v>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>σ_t(Прямая)</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -2768,57 +2704,10 @@
       <c r="H118" t="n">
         <v>1310.4</v>
       </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="B119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="C119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="D119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="E119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="F119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="G119" t="n">
-        <v>3994.01</v>
-      </c>
-      <c r="H119" t="n">
-        <v>3994.01</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="B120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="C120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="D120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="E120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="F120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="G120" t="n">
-        <v>3997.04</v>
-      </c>
-      <c r="H120" t="n">
-        <v>3997.04</v>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>σ_t(Кривая)</t>
+        </is>
       </c>
     </row>
     <row r="121">
@@ -2846,6 +2735,11 @@
       <c r="H121" t="n">
         <v>1909.24</v>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>σ_кп^зима_ПРямая</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2872,6 +2766,11 @@
       <c r="H122" t="n">
         <v>2066.65</v>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>σ_кп^зима_Кривая</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2898,6 +2797,11 @@
       <c r="H123" t="n">
         <v>3161.93</v>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>критическая температурная сила Pк(Прямая)</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2924,6 +2828,11 @@
       <c r="H124" t="n">
         <v>2016.18</v>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>критическая температурная сила Pк(Кривая)</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2950,6 +2859,11 @@
       <c r="H125" t="n">
         <v>322427.13</v>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>Pк(Прямая)кгс</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2976,6 +2890,11 @@
       <c r="H126" t="n">
         <v>205593.14</v>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>Pк(Кривая)кгс</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -3002,6 +2921,11 @@
       <c r="H127" t="n">
         <v>214951.42</v>
       </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>[P]Прямая</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -3028,6 +2952,11 @@
       <c r="H128" t="n">
         <v>137062.09</v>
       </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>[P]Кривая</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -3054,6 +2983,11 @@
       <c r="H129" t="n">
         <v>65.98999999999999</v>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -3080,6 +3014,11 @@
       <c r="H130" t="n">
         <v>131.98</v>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>F * 2</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -3106,6 +3045,11 @@
       <c r="H131" t="n">
         <v>65.15000000000001</v>
       </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>[∆t_у0]</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -3132,125 +3076,130 @@
       <c r="H132" t="n">
         <v>41.54</v>
       </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>[∆t_у0]</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; η = -0.04017
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; η = 0</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; η = -0.0277
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; η = 0</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; η = -0.03826
-III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; η = 0
-VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; η = 0</t>
-        </is>
-      </c>
-      <c r="D133" t="inlineStr">
         <is>
           <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
 III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
 VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
+        </is>
+      </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>I ось: x = 185 см; kx = 0.01145×185 = 2.12; η = 0.04008
-III ось: x = 125 см; kx = 0.01145×125 = 1.43; η = 0.26993
-VI ось: x = 125+185 см; kx = 0.01145×310 = 3.55; η = -0.03778</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>I ось: x = 185 см; kx = 0.01311×185 = 2.43; η = -0.00864
-III ось: x = 125 см; kx = 0.01311×125 = 1.64; η = 0.18059
-VI ось: x = 125+185 см; kx = 0.01311×310 = 4.06; η = -0.02407</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>I ось: x = 185 см; kx = 0.01176×185 = 2.18; η = 0.02884
-III ось: x = 125 см; kx = 0.01176×125 = 1.47; η = 0.25189
-VI ось: x = 125+185 см; kx = 0.01176×310 = 3.65; η = -0.03547</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>I ось: x = 185 см; kx = 0.01372×185 = 2.54; η = -0.02022
-III ось: x = 125 см; kx = 0.01372×125 = 1.71; η = 0.15223
-VI ось: x = 125+185 см; kx = 0.01372×310 = 4.25; η = -0.01905</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; η = -0.02265
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; η = 0
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; η = 0</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01145×300 = 3.44; µ = -0.02153
-III ось: x = 0+300 см; kx = 0.01145×300 = 3.44; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01145×300 = 3.44; µ = 0.00000</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01311×300 = 3.93; µ = 0.00017
-III ось: x = 0+300 см; kx = 0.01311×300 = 3.93; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01311×300 = 3.93; µ = 0.00000</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>II ось: x = 300 см; kx = 0.01176×300 = 3.53; µ = -0.01613
-III ось: x = 0+300 см; kx = 0.01176×300 = 3.53; µ = 0.00000
-VI ось: x = 300+0+0 см; kx = 0.01176×300 = 3.53; µ = 0.00000</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
         <is>
           <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
 III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
 VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
+        </is>
+      </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>II ось: x = 185 см; kx = 0.01145×185 = 2.12; µ = -0.16526
-III ось: x = 125+185 см; kx = 0.01145×310 = 3.55; µ = -0.01498
-VI ось: x = 185+125+185 см; kx = 0.01145×495 = 5.67; µ = 0.00000</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>II ось: x = 185 см; kx = 0.01311×185 = 2.43; µ = -0.12478
-III ось: x = 125+185 см; kx = 0.01311×310 = 4.06; µ = 0.00332
-VI ось: x = 185+125+185 см; kx = 0.01311×495 = 6.49; µ = 0.00000</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>II ось: x = 185 см; kx = 0.01176×185 = 2.18; µ = -0.15796
-III ось: x = 125+185 см; kx = 0.01176×310 = 3.65; µ = -0.01025
-VI ось: x = 185+125+185 см; kx = 0.01176×495 = 5.82; µ = 0.00000</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>II ось: x = 185 см; kx = 0.01372×185 = 2.54; µ = -0.10989
-III ось: x = 125+185 см; kx = 0.01372×310 = 4.25; µ = 0.00644
-VI ось: x = 185+125+185 см; kx = 0.01372×495 = 6.79; µ = 0.00000</t>
+          <t>II ось: x = 300 см; kx = 0.01372×300 = 4.12; µ = 0.00433
+III ось: x = 0+300 см; kx = 0.01372×300 = 4.12; µ = 0.00000
+VI ось: x = 300+0+0 см; kx = 0.01372×300 = 4.12; µ = 0.00000</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="E135" t="inlineStr">
+      <c r="A135" t="inlineStr">
         <is>
           <t>ηI: x = 185 - 55 см; kx = 0.01145×130 = 1.49; η = 0.04008
 ηII: x = 55 см; kx = 0.01145×55 = 0.63; η = 0.74428
@@ -3258,28 +3207,9 @@
 ηIV: x = 125+185+55; kx = 0.01145×365 = 3.61; η = -0.02097</t>
         </is>
       </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>ηI: x = 185 - 55 см; kx = 0.01311×130 = 1.70; η = -0.00864
-ηII: x = 55 см; kx = 0.01311×55 = 0.72; η = 0.68623
-ηIII: x = 125+55 см; kx = 0.01311×180 = 56.64; η = -0.00048
-ηIV: x = 125+185+55; kx = 0.01311×365 = 4.13; η = -0.00772</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>ηI: x = 185 - 55 см; kx = 0.01176×130 = 1.53; η = 0.02884
-ηII: x = 55 см; kx = 0.01176×55 = 0.65; η = 0.73355
-ηIII: x = 125+55 см; kx = 0.01176×180 = 56.47; η = 0.04038
-ηIV: x = 125+185+55; kx = 0.01176×365 = 3.70; η = -0.01806</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
-        <is>
-          <t>ηI: x = 185 - 55 см; kx = 0.01372×130 = 1.78; η = -0.02022
-ηII: x = 55 см; kx = 0.01372×55 = 0.75; η = 0.66465
-ηIII: x = 125+55 см; kx = 0.01372×180 = 56.72; η = -0.01354
-ηIV: x = 125+185+55; kx = 0.01372×365 = 4.32; η = -0.00445</t>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>Ekv_gruzi_η_shpala_1</t>
         </is>
       </c>
     </row>

</xml_diff>